<commit_message>
added "back to home" hyperlinks
</commit_message>
<xml_diff>
--- a/scores.xlsx
+++ b/scores.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t xml:space="preserve">Unnamed: 0</t>
+  </si>
   <si>
     <t xml:space="preserve">#Ronde</t>
   </si>
@@ -131,17 +134,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -336,10 +335,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -366,12 +365,18 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -379,7 +384,10 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -387,7 +395,10 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="0" t="n">
         <v>3</v>
       </c>
     </row>
@@ -395,7 +406,10 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="n">
         <v>4</v>
       </c>
     </row>
@@ -403,7 +417,10 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="0" t="n">
         <v>5</v>
       </c>
     </row>
@@ -411,7 +428,10 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="0" t="n">
         <v>6</v>
       </c>
     </row>
@@ -419,7 +439,10 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="0" t="n">
         <v>7</v>
       </c>
     </row>
@@ -427,7 +450,10 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" s="0" t="n">
         <v>8</v>
       </c>
     </row>
@@ -435,7 +461,10 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" s="0" t="n">
         <v>9</v>
       </c>
     </row>
@@ -443,7 +472,10 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" s="0" t="n">
         <v>10</v>
       </c>
     </row>
@@ -451,7 +483,10 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" s="0" t="n">
         <v>11</v>
       </c>
     </row>
@@ -459,7 +494,10 @@
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C13" s="0" t="n">
         <v>12</v>
       </c>
     </row>
@@ -467,7 +505,10 @@
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C14" s="0" t="n">
         <v>13</v>
       </c>
     </row>
@@ -475,7 +516,10 @@
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C15" s="0" t="n">
         <v>14</v>
       </c>
     </row>
@@ -483,7 +527,10 @@
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C16" s="0" t="n">
         <v>15</v>
       </c>
     </row>
@@ -491,7 +538,10 @@
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B17" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C17" s="0" t="n">
         <v>16</v>
       </c>
     </row>
@@ -499,7 +549,10 @@
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B18" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C18" s="0" t="n">
         <v>17</v>
       </c>
     </row>
@@ -507,7 +560,10 @@
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C19" s="0" t="n">
         <v>18</v>
       </c>
     </row>
@@ -515,7 +571,10 @@
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="n">
+      <c r="B20" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C20" s="0" t="n">
         <v>19</v>
       </c>
     </row>
@@ -523,7 +582,10 @@
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" s="2" t="n">
+      <c r="B21" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C21" s="0" t="n">
         <v>20</v>
       </c>
     </row>

</xml_diff>